<commit_message>
Fix error: tried to save LineString with null Value (it's required) #86
</commit_message>
<xml_diff>
--- a/ElectionStatistics.Tests/Resources/import_data.xlsx
+++ b/ElectionStatistics.Tests/Resources/import_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="92">
   <si>
     <t xml:space="preserve">link</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t xml:space="preserve">УИК №402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.udmurt.vybory.izbirkom.ru/region/udmurt?action=show&amp;global=true&amp;root=184002039&amp;tvd=4184002259111&amp;vrn=100100084849062&amp;prver=0&amp;pronetvd=null&amp;region=18&amp;sub_region=18&amp;type=226&amp;vibid=4184002259111</t>
   </si>
   <si>
     <t xml:space="preserve">Удмуртская Республика</t>
@@ -334,6 +331,7 @@
       <sz val="10"/>
       <name val="PingFang SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -411,7 +409,7 @@
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD40" activeCellId="0" sqref="AD40"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1863,20 +1861,17 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="B18" s="0" t="n">
         <v>1139</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>3</v>
@@ -1942,24 +1937,24 @@
         <v>0</v>
       </c>
       <c r="AC18" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1212</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>3</v>
@@ -2025,21 +2020,21 @@
         <v>1</v>
       </c>
       <c r="AC19" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1140</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>3</v>
@@ -2105,24 +2100,24 @@
         <v>0</v>
       </c>
       <c r="AC20" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1141</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="E21" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>3</v>
@@ -2188,24 +2183,24 @@
         <v>7</v>
       </c>
       <c r="AC21" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1213</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>3</v>
@@ -2271,24 +2266,24 @@
         <v>0</v>
       </c>
       <c r="AC22" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1142</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>3</v>
@@ -2354,27 +2349,27 @@
         <v>0</v>
       </c>
       <c r="AC23" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AD23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1204</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>9</v>
@@ -2437,30 +2432,30 @@
         <v>5</v>
       </c>
       <c r="AB24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC24" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="AC24" s="0" t="s">
+      <c r="AD24" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>63</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="E26" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>5</v>
@@ -2526,27 +2521,27 @@
         <v>9</v>
       </c>
       <c r="AC26" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD26" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AD26" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1206</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="E27" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>9</v>
@@ -2612,27 +2607,27 @@
         <v>1</v>
       </c>
       <c r="AC27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD27" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="AD27" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>918</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>8</v>
@@ -2698,50 +2693,50 @@
         <v>0</v>
       </c>
       <c r="AC28" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1208</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="E29" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>9</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC29" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1207</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="E30" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>9</v>
@@ -2807,18 +2802,18 @@
         <v>2</v>
       </c>
       <c r="AC30" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>9</v>
@@ -2884,7 +2879,7 @@
         <v>2</v>
       </c>
       <c r="AC31" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,16 +2951,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1207</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>1071</v>
@@ -3030,16 +3025,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>12555</v>
       </c>
       <c r="D35" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>1071</v>

</xml_diff>

<commit_message>
Import: infer string values out of any type #88
</commit_message>
<xml_diff>
--- a/ElectionStatistics.Tests/Resources/import_data.xlsx
+++ b/ElectionStatistics.Tests/Resources/import_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
   <si>
     <t xml:space="preserve">link</t>
   </si>
@@ -79,9 +79,6 @@
     <t xml:space="preserve">УИК №1413</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.tula.vybory.izbirkom.ru/region/tula?action=show&amp;global=true&amp;root=714014014&amp;tvd=4714014146702&amp;vrn=100100084849062&amp;prver=0&amp;pronetvd=null&amp;region=71&amp;sub_region=71&amp;type=226&amp;vibid=4714014146702</t>
-  </si>
-  <si>
     <t xml:space="preserve">УИК №1414</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t xml:space="preserve">УИК №1601</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.tula.vybory.izbirkom.ru/region/tula?action=show&amp;global=true&amp;root=714016002&amp;tvd=4714016254742&amp;vrn=100100084849062&amp;prver=0&amp;pronetvd=null&amp;region=71&amp;sub_region=71&amp;type=226&amp;vibid=4714016254742</t>
-  </si>
-  <si>
     <t xml:space="preserve">УИК №1602</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">УИК №102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.tyumen.vybory.izbirkom.ru/region/tyumen?action=show&amp;global=true&amp;root=724001003&amp;tvd=4724001161251&amp;vrn=100100084849062&amp;prver=0&amp;pronetvd=null&amp;region=72&amp;sub_region=72&amp;type=226&amp;vibid=4724001161251</t>
   </si>
   <si>
     <t xml:space="preserve">УИК №103</t>
@@ -302,8 +293,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MMM\ D&quot;, &quot;YY"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -376,12 +369,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,7 +410,7 @@
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,8 +863,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>19</v>
+      <c r="A6" s="0" t="n">
+        <v>3344</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1414</v>
@@ -875,7 +876,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>1</v>
@@ -946,7 +947,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1501</v>
@@ -955,10 +956,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1</v>
@@ -1029,7 +1030,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1502</v>
@@ -1038,10 +1039,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
@@ -1112,7 +1113,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1601</v>
@@ -1121,10 +1122,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -1194,8 +1195,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>29</v>
+      <c r="A10" s="1" t="n">
+        <v>43809</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1602</v>
@@ -1204,10 +1205,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1</v>
@@ -1278,7 +1279,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1603</v>
@@ -1287,10 +1288,10 @@
         <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1</v>
@@ -1361,19 +1362,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>101</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>22</v>
@@ -1439,27 +1440,27 @@
         <v>5</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>102</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>22</v>
@@ -1525,24 +1526,24 @@
         <v>1</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>41</v>
+      <c r="A14" s="3" t="n">
+        <v>100</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>103</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>22</v>
@@ -1605,24 +1606,24 @@
         <v>4</v>
       </c>
       <c r="AC14" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>104</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>22</v>
@@ -1688,24 +1689,24 @@
         <v>0</v>
       </c>
       <c r="AC15" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>401</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>22</v>
@@ -1771,24 +1772,24 @@
         <v>0</v>
       </c>
       <c r="AC16" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>402</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>22</v>
@@ -1854,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="AC17" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,13 +1863,13 @@
         <v>1139</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>3</v>
@@ -1934,24 +1935,24 @@
         <v>0</v>
       </c>
       <c r="AC18" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1212</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>3</v>
@@ -2017,21 +2018,21 @@
         <v>1</v>
       </c>
       <c r="AC19" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1140</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>3</v>
@@ -2094,24 +2095,24 @@
         <v>0</v>
       </c>
       <c r="AC20" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1141</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>3</v>
@@ -2177,24 +2178,24 @@
         <v>7</v>
       </c>
       <c r="AC21" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1213</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>3</v>
@@ -2260,24 +2261,24 @@
         <v>0</v>
       </c>
       <c r="AC22" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1142</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>3</v>
@@ -2343,27 +2344,27 @@
         <v>0</v>
       </c>
       <c r="AC23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1204</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>9</v>
@@ -2426,30 +2427,30 @@
         <v>5</v>
       </c>
       <c r="AB24" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AC24" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>63</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>5</v>
@@ -2515,27 +2516,27 @@
         <v>9</v>
       </c>
       <c r="AC26" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD26" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1206</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>9</v>
@@ -2601,27 +2602,27 @@
         <v>1</v>
       </c>
       <c r="AC27" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD27" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="AD27" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>918</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>8</v>
@@ -2687,50 +2688,50 @@
         <v>0</v>
       </c>
       <c r="AC28" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1208</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>9</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AC29" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1207</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>9</v>
@@ -2796,18 +2797,18 @@
         <v>2</v>
       </c>
       <c r="AC30" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>9</v>
@@ -2873,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="AC31" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,16 +2946,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1207</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>1071</v>
@@ -3019,16 +3020,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="B35" s="4" t="n">
         <v>12555</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>1071</v>

</xml_diff>

<commit_message>
LDA: use ADO for raw sql queries #93
LDA: fully migrate to ADO #93
</commit_message>
<xml_diff>
--- a/ElectionStatistics.Tests/Resources/import_data.xlsx
+++ b/ElectionStatistics.Tests/Resources/import_data.xlsx
@@ -295,7 +295,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MMM\ D&quot;, &quot;YY"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="5">
@@ -410,7 +410,7 @@
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>43809</v>
+        <v>0.93</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1602</v>

</xml_diff>